<commit_message>
Updated lineage checks with geo data
</commit_message>
<xml_diff>
--- a/checks/results/HLR_results_1_Dunn_lgs_tPBC.xlsx
+++ b/checks/results/HLR_results_1_Dunn_lgs_tPBC.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Model Level</t>
   </si>
@@ -85,64 +85,85 @@
     <t>['N1ratio-ArgsPreds']</t>
   </si>
   <si>
-    <t>['N1ratio-ArgsPreds', 'Nlen_freq', 'Vlen_freq']</t>
-  </si>
-  <si>
-    <t>['N1ratio-ArgsPreds', 'Nlen_freq', 'Vlen_freq', 'Fam_class']</t>
-  </si>
-  <si>
-    <t>{'const': 0.8769068789051704, 'N1ratio-ArgsPreds': -0.2589207324877432}</t>
-  </si>
-  <si>
-    <t>{'const': 0.5801195161575956, 'N1ratio-ArgsPreds': -0.25331948949682775, 'Nlen_freq': -0.014596167007057292, 'Vlen_freq': 0.05913663318206994}</t>
-  </si>
-  <si>
-    <t>{'const': 0.5631272161868974, 'N1ratio-ArgsPreds': -0.2510006127729462, 'Nlen_freq': -0.00863388669301103, 'Vlen_freq': 0.05687208891707852, 'Fam_class': -0.0003911008749667151}</t>
-  </si>
-  <si>
-    <t>{'const': 3.726577191319948e-15, 'N1ratio-ArgsPreds': 7.810452239193888e-10}</t>
-  </si>
-  <si>
-    <t>{'const': 0.039630138651555145, 'N1ratio-ArgsPreds': 3.2882260031291886e-09, 'Nlen_freq': 0.805842553341692, 'Vlen_freq': 0.24338667875661385}</t>
-  </si>
-  <si>
-    <t>{'const': 0.05144489288927981, 'N1ratio-ArgsPreds': 9.292963778163899e-09, 'Nlen_freq': 0.8912076434730541, 'Vlen_freq': 0.26956854244675243, 'Fam_class': 0.772917792296008}</t>
-  </si>
-  <si>
-    <t>{'N1ratio-ArgsPreds': -0.553136892881466}</t>
-  </si>
-  <si>
-    <t>{'N1ratio-ArgsPreds': -0.5411708594375596, 'Nlen_freq': -0.0296241065201804, 'Vlen_freq': 0.14075734002025153}</t>
-  </si>
-  <si>
-    <t>{'N1ratio-ArgsPreds': -0.5362170025034352, 'Nlen_freq': -0.017523174334279724, 'Vlen_freq': 0.1353672592877733, 'Fam_class': -0.02613956669393624}</t>
+    <t>['N1ratio-ArgsPreds', 'latitude', 'longitude', 'Macro_class']</t>
+  </si>
+  <si>
+    <t>['N1ratio-ArgsPreds', 'latitude', 'longitude', 'Macro_class', 'Fam_class']</t>
+  </si>
+  <si>
+    <t>['N1ratio-ArgsPreds', 'latitude', 'longitude', 'Macro_class', 'Fam_class', 'Nlen_freq', 'Vlen_freq']</t>
+  </si>
+  <si>
+    <t>{'const': 0.8769068789051704, 'N1ratio-ArgsPreds': -0.25892073248774317}</t>
+  </si>
+  <si>
+    <t>{'const': 0.492442807410804, 'N1ratio-ArgsPreds': -0.2347084757011529, 'latitude': -0.00039709861635979916, 'longitude': -0.0005177668538437926, 'Macro_class': 0.13581942809818}</t>
+  </si>
+  <si>
+    <t>{'const': 0.6390956805391714, 'N1ratio-ArgsPreds': -0.22578922616158928, 'latitude': -0.000525123248977932, 'longitude': -0.0010411331253083384, 'Macro_class': 0.11757684971827578, 'Fam_class': -0.002279536807291503}</t>
+  </si>
+  <si>
+    <t>{'const': 0.07174266864899048, 'N1ratio-ArgsPreds': -0.22105968489772074, 'latitude': 0.0002667620768122055, 'longitude': -0.0013574861844785654, 'Macro_class': 0.10147993435936434, 'Fam_class': -0.0047730797442657015, 'Nlen_freq': 0.06963180770116814, 'Vlen_freq': 0.0385371271582626}</t>
+  </si>
+  <si>
+    <t>{'const': 3.726577191319948e-15, 'N1ratio-ArgsPreds': 7.810452239194086e-10}</t>
+  </si>
+  <si>
+    <t>{'const': 7.325298994937364e-05, 'N1ratio-ArgsPreds': 1.3185501625227715e-09, 'latitude': 0.787682088353225, 'longitude': 0.24372793217946584, 'Macro_class': 2.2147465213834944e-06}</t>
+  </si>
+  <si>
+    <t>{'const': 0.0002704792054073951, 'N1ratio-ArgsPreds': 7.841109645115831e-09, 'latitude': 0.7218232433499598, 'longitude': 0.09398637531538649, 'Macro_class': 0.00024134675563298213, 'Fam_class': 0.22666500312154214}</t>
+  </si>
+  <si>
+    <t>{'const': 0.7972316822536156, 'N1ratio-ArgsPreds': 1.2220126715507334e-08, 'latitude': 0.8567082391104337, 'longitude': 0.029702017900401882, 'Macro_class': 0.0013936046111223586, 'Fam_class': 0.025601998533392043, 'Nlen_freq': 0.23396876351533552, 'Vlen_freq': 0.3983691468942224}</t>
+  </si>
+  <si>
+    <t>{'N1ratio-ArgsPreds': -0.5531368928814658}</t>
+  </si>
+  <si>
+    <t>{'N1ratio-ArgsPreds': -0.5014118249044676, 'latitude': -0.022114931134383408, 'longitude': -0.10051783646596273, 'Macro_class': 0.39915299056925585}</t>
+  </si>
+  <si>
+    <t>{'N1ratio-ArgsPreds': -0.48235747599333034, 'latitude': -0.02924478708756917, 'longitude': -0.2021227285063198, 'Macro_class': 0.3455407804606315, 'Fam_class': -0.157703905320072}</t>
+  </si>
+  <si>
+    <t>{'N1ratio-ArgsPreds': -0.47225367420691, 'latitude': 0.014856322119797389, 'longitude': -0.26353864347096045, 'Macro_class': 0.2982343531371035, 'Fam_class': -0.3302132756387528, 'Nlen_freq': 0.14132340960025755, 'Vlen_freq': 0.09172628232179939}</t>
+  </si>
+  <si>
+    <t>{'N1ratio-ArgsPreds': -0.5531368928814663}</t>
+  </si>
+  <si>
+    <t>{'N1ratio-ArgsPreds': -0.5536010432239684, 'latitude': -0.026860080239888274, 'longitude': -0.11588859139307682, 'Macro_class': 0.4469540976552578}</t>
+  </si>
+  <si>
+    <t>{'N1ratio-ArgsPreds': -0.5333790629645466, 'latitude': -0.035680055520583905, 'longitude': -0.16671544191102688, 'Macro_class': 0.35591767925655415, 'Fam_class': -0.12075793785607132}</t>
+  </si>
+  <si>
+    <t>{'N1ratio-ArgsPreds': -0.5320484327264897, 'latitude': 0.018284980288520318, 'longitude': -0.21752858914027481, 'Macro_class': 0.3153651815706621, 'Fam_class': -0.22320178764535017, 'Nlen_freq': 0.12009834319405689, 'Vlen_freq': 0.08537275883833031}</t>
   </si>
   <si>
     <t>{'N1ratio-ArgsPreds': -0.5531368928814662}</t>
   </si>
   <si>
-    <t>{'N1ratio-ArgsPreds': -0.5400522781546515, 'Nlen_freq': -0.024393212816919203, 'Vlen_freq': 0.11540310277040416}</t>
-  </si>
-  <si>
-    <t>{'N1ratio-ArgsPreds': -0.5289082141371704, 'Nlen_freq': -0.01364284049686088, 'Vlen_freq': 0.1097966418844574, 'Fam_class': -0.02877802668041927}</t>
-  </si>
-  <si>
-    <t>{'N1ratio-ArgsPreds': -0.5531368928814664}</t>
-  </si>
-  <si>
-    <t>{'N1ratio-ArgsPreds': -0.5289440201292877, 'Nlen_freq': -0.020113800078406772, 'Vlen_freq': 0.09576895148458565}</t>
-  </si>
-  <si>
-    <t>{'N1ratio-ArgsPreds': -0.5135146116515139, 'Nlen_freq': -0.011242455806926399, 'Vlen_freq': 0.09102039310397214, 'Fam_class': -0.02372230513956744}</t>
-  </si>
-  <si>
-    <t>{'N1ratio-ArgsPreds': 30.596042226656284}</t>
-  </si>
-  <si>
-    <t>{'N1ratio-ArgsPreds': 27.978177643053225, 'Nlen_freq': 0.04045649535941163, 'Vlen_freq': 0.9171692068456921}</t>
-  </si>
-  <si>
-    <t>{'N1ratio-ArgsPreds': 26.36972563796051, 'Nlen_freq': 0.012639281257069312, 'Vlen_freq': 0.8284711960801618, 'Fam_class': 0.05627477611347477}</t>
+    <t>{'N1ratio-ArgsPreds': -0.49437227359470837, 'latitude': -0.019982626440729546, 'longitude': -0.08676914369418048, 'Macro_class': 0.37157244508480686}</t>
+  </si>
+  <si>
+    <t>{'N1ratio-ArgsPreds': -0.46550866799422724, 'latitude': -0.026357294175478444, 'longitude': -0.12482321704588047, 'Macro_class': 0.2811647640366989, 'Fam_class': -0.08980576808409556}</t>
+  </si>
+  <si>
+    <t>{'N1ratio-ArgsPreds': -0.44915676676172267, 'latitude': 0.01307225734629092, 'longitude': -0.159303749956017, 'Macro_class': 0.2375442705402404, 'Fam_class': -0.16367335530192872, 'Nlen_freq': 0.08647196942162136, 'Vlen_freq': 0.06124790955740818}</t>
+  </si>
+  <si>
+    <t>{'N1ratio-ArgsPreds': 30.596042226656255}</t>
+  </si>
+  <si>
+    <t>{'N1ratio-ArgsPreds': 24.440394489920116, 'latitude': 0.03993053594697436, 'longitude': 0.7528884297421341, 'Macro_class': 13.80660819463018}</t>
+  </si>
+  <si>
+    <t>{'N1ratio-ArgsPreds': 21.66983199777597, 'latitude': 0.069470695625271, 'longitude': 1.5580835513682985, 'Macro_class': 7.905362453581256, 'Fam_class': 0.8065075981174357}</t>
+  </si>
+  <si>
+    <t>{'N1ratio-ArgsPreds': 20.174180112784455, 'latitude': 0.017088391212765692, 'longitude': 2.537768475004919, 'Macro_class': 5.642728046649493, 'Fam_class': 2.67889672357914, 'Nlen_freq': 0.7477401495653819, 'Vlen_freq': 0.3751306425152452}</t>
   </si>
 </sst>
 </file>
@@ -500,7 +521,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W4"/>
+  <dimension ref="A1:W5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -594,46 +615,46 @@
         <v>1</v>
       </c>
       <c r="G2">
-        <v>0.3059604222665625</v>
+        <v>0.3059604222665624</v>
       </c>
       <c r="H2">
-        <v>45.84736222052123</v>
+        <v>45.84736222052121</v>
       </c>
       <c r="I2">
-        <v>7.81045223919384E-10</v>
+        <v>7.810452239193906E-10</v>
       </c>
       <c r="J2">
-        <v>14.92839846445507</v>
+        <v>14.92839846445508</v>
       </c>
       <c r="K2">
         <v>21.50943396226416</v>
       </c>
       <c r="L2">
-        <v>6.581035497809083</v>
+        <v>6.581035497809081</v>
       </c>
       <c r="M2">
-        <v>0.1435422929274526</v>
+        <v>0.1435422929274527</v>
       </c>
       <c r="N2">
         <v>0.2048517520215634</v>
       </c>
       <c r="O2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="P2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="Q2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="R2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="S2" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="T2" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:23">
@@ -650,61 +671,61 @@
         <v>106</v>
       </c>
       <c r="E3">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G3">
-        <v>0.3204964123472243</v>
+        <v>0.4469338392920367</v>
       </c>
       <c r="H3">
-        <v>16.03652757367618</v>
+        <v>20.4045740706288</v>
       </c>
       <c r="I3">
-        <v>1.296295875620921E-08</v>
+        <v>2.413267169335551E-12</v>
       </c>
       <c r="J3">
-        <v>14.61573754573895</v>
+        <v>11.89614006051091</v>
       </c>
       <c r="K3">
         <v>21.50943396226416</v>
       </c>
       <c r="L3">
-        <v>2.297898805508401</v>
+        <v>2.403323475438311</v>
       </c>
       <c r="M3">
-        <v>0.1432915445660682</v>
+        <v>0.1177835649555536</v>
       </c>
       <c r="N3">
         <v>0.2048517520215634</v>
       </c>
       <c r="O3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="Q3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="R3" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="S3" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="T3" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="U3">
-        <v>0.01453599008066175</v>
+        <v>0.1409734170254743</v>
       </c>
       <c r="V3">
-        <v>1.090995702722573</v>
+        <v>8.581441746105543</v>
       </c>
       <c r="W3">
-        <v>0.3397687062236793</v>
+        <v>3.955623329731498E-05</v>
       </c>
     </row>
     <row r="4" spans="1:23">
@@ -721,61 +742,132 @@
         <v>106</v>
       </c>
       <c r="E4">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G4">
-        <v>0.321059160108359</v>
+        <v>0.454998915273213</v>
       </c>
       <c r="H4">
-        <v>11.94028008983802</v>
+        <v>16.69717466714061</v>
       </c>
       <c r="I4">
-        <v>5.538364082825791E-08</v>
+        <v>5.794027875875511E-12</v>
       </c>
       <c r="J4">
-        <v>14.60363315993341</v>
+        <v>11.72266484129316</v>
       </c>
       <c r="K4">
         <v>21.50943396226416</v>
       </c>
       <c r="L4">
-        <v>1.726450200582686</v>
+        <v>1.9573538241942</v>
       </c>
       <c r="M4">
-        <v>0.1445904273260734</v>
+        <v>0.1172266484129316</v>
       </c>
       <c r="N4">
         <v>0.2048517520215634</v>
       </c>
       <c r="O4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="Q4" t="s">
+        <v>36</v>
+      </c>
+      <c r="R4" t="s">
+        <v>40</v>
+      </c>
+      <c r="S4" t="s">
+        <v>44</v>
+      </c>
+      <c r="T4" t="s">
+        <v>48</v>
+      </c>
+      <c r="U4">
+        <v>0.00806507598117634</v>
+      </c>
+      <c r="V4">
+        <v>1.479827509924943</v>
+      </c>
+      <c r="W4">
+        <v>0.2266650031215442</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5">
+        <v>106</v>
+      </c>
+      <c r="E5">
+        <v>98</v>
+      </c>
+      <c r="F5">
+        <v>7</v>
+      </c>
+      <c r="G5">
+        <v>0.4890634649576791</v>
+      </c>
+      <c r="H5">
+        <v>13.40066336974782</v>
+      </c>
+      <c r="I5">
+        <v>4.989964903313639E-12</v>
+      </c>
+      <c r="J5">
+        <v>10.98995565940087</v>
+      </c>
+      <c r="K5">
+        <v>21.50943396226416</v>
+      </c>
+      <c r="L5">
+        <v>1.502782614694755</v>
+      </c>
+      <c r="M5">
+        <v>0.112142404687764</v>
+      </c>
+      <c r="N5">
+        <v>0.2048517520215634</v>
+      </c>
+      <c r="O5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P5" t="s">
         <v>33</v>
       </c>
-      <c r="R4" t="s">
-        <v>36</v>
-      </c>
-      <c r="S4" t="s">
-        <v>39</v>
-      </c>
-      <c r="T4" t="s">
-        <v>42</v>
-      </c>
-      <c r="U4">
-        <v>0.0005627477611347409</v>
-      </c>
-      <c r="V4">
-        <v>0.0837149874261211</v>
-      </c>
-      <c r="W4">
-        <v>0.7729177922962384</v>
+      <c r="Q5" t="s">
+        <v>37</v>
+      </c>
+      <c r="R5" t="s">
+        <v>41</v>
+      </c>
+      <c r="S5" t="s">
+        <v>45</v>
+      </c>
+      <c r="T5" t="s">
+        <v>49</v>
+      </c>
+      <c r="U5">
+        <v>0.03406454968446604</v>
+      </c>
+      <c r="V5">
+        <v>3.266869405611362</v>
+      </c>
+      <c r="W5">
+        <v>0.042316525175481</v>
       </c>
     </row>
   </sheetData>

</xml_diff>